<commit_message>
session 0 patch, fighter
</commit_message>
<xml_diff>
--- a/Monster Manual.xlsx
+++ b/Monster Manual.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="576" yWindow="348" windowWidth="20724" windowHeight="9756"/>
+    <workbookView xWindow="576" yWindow="348" windowWidth="20724" windowHeight="9756" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Elk" sheetId="1" r:id="rId1"/>
+    <sheet name="Skeletons" sheetId="2" r:id="rId1"/>
+    <sheet name="Elk" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="55">
   <si>
     <t>Elk</t>
   </si>
@@ -40,9 +41,6 @@
     <t>CHA</t>
   </si>
   <si>
-    <t>Hooves x1</t>
-  </si>
-  <si>
     <t>Hit Points</t>
   </si>
   <si>
@@ -58,13 +56,130 @@
     <t>CR</t>
   </si>
   <si>
-    <t>Charge x2</t>
+    <t>Dodge x3</t>
+  </si>
+  <si>
+    <t>0.25 (50 XP)</t>
+  </si>
+  <si>
+    <t>Senses</t>
+  </si>
+  <si>
+    <t>Perception 10</t>
+  </si>
+  <si>
+    <t>Skeleton</t>
+  </si>
+  <si>
+    <t>Medium undead, lawful evil</t>
+  </si>
+  <si>
+    <t>30 ft.</t>
+  </si>
+  <si>
+    <t>Vulnerabilities</t>
+  </si>
+  <si>
+    <t>bludgeoning</t>
+  </si>
+  <si>
+    <t>Immunities</t>
+  </si>
+  <si>
+    <t>poison, exhaustion</t>
+  </si>
+  <si>
+    <t>Languages</t>
+  </si>
+  <si>
+    <t>understands all languages it knew in life, but can't speak</t>
+  </si>
+  <si>
+    <t>Block x2</t>
+  </si>
+  <si>
+    <t>Armor scraps</t>
+  </si>
+  <si>
+    <t>Minotaur Skeleton</t>
+  </si>
+  <si>
+    <t>Large undead, lawful evil</t>
+  </si>
+  <si>
+    <t>darkvision, perception 9</t>
+  </si>
+  <si>
+    <t>perception 9</t>
+  </si>
+  <si>
+    <t>(2d10 + 2)</t>
+  </si>
+  <si>
+    <t>(2d8 + 4)</t>
+  </si>
+  <si>
+    <t>(9d10 + 18)</t>
+  </si>
+  <si>
+    <t>understands Abyssal but can't speak</t>
+  </si>
+  <si>
+    <t>2 (450 XP)</t>
+  </si>
+  <si>
+    <t>Hooves x2</t>
+  </si>
+  <si>
+    <t>Strike x6</t>
+  </si>
+  <si>
+    <t>Shortsword (piercing)</t>
+  </si>
+  <si>
+    <t>Shortbow (piercing)</t>
+  </si>
+  <si>
+    <t>Greataxe (slashing)</t>
+  </si>
+  <si>
+    <t>Hand Size</t>
+  </si>
+  <si>
+    <t>Hooves x3</t>
+  </si>
+  <si>
+    <t>Parry x2</t>
+  </si>
+  <si>
+    <t>Shoot x4</t>
+  </si>
+  <si>
+    <t>Dodge x2</t>
+  </si>
+  <si>
+    <t>Shortsword</t>
+  </si>
+  <si>
+    <t>Strike+ x6</t>
+  </si>
+  <si>
+    <t>Strike+ x8</t>
+  </si>
+  <si>
+    <t>Example Deck</t>
+  </si>
+  <si>
+    <t>Gore x4</t>
+  </si>
+  <si>
+    <t>Shatter x2</t>
+  </si>
+  <si>
+    <t>Charge x3</t>
   </si>
   <si>
     <t>Ram x6</t>
-  </si>
-  <si>
-    <t>Dodge x3</t>
   </si>
 </sst>
 </file>
@@ -125,11 +240,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,13 +540,352 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="13.77734375" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="3"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <v>18</v>
+      </c>
+      <c r="K5">
+        <v>11</v>
+      </c>
+      <c r="L5">
+        <v>15</v>
+      </c>
+      <c r="M5">
+        <v>6</v>
+      </c>
+      <c r="N5">
+        <v>8</v>
+      </c>
+      <c r="O5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7">
+        <v>67</v>
+      </c>
+      <c r="L7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="J17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="J18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="J19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="J20" t="s">
+        <v>48</v>
+      </c>
+      <c r="L20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="J21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="J23" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="J24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="J25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="J26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="J27" t="s">
+        <v>49</v>
+      </c>
+      <c r="L27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="J28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
@@ -447,94 +902,125 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>16</v>
+      </c>
+      <c r="B5">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="3"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1" t="s">
+      <c r="C5">
+        <v>12</v>
+      </c>
+      <c r="D5">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5">
         <v>6</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7">
-        <v>16</v>
+      <c r="A7" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B7">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
         <v>10</v>
-      </c>
-      <c r="C7">
-        <v>12</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>10</v>
-      </c>
-      <c r="F7">
-        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9">
-        <v>0.25</v>
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
         <v>15</v>
       </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>16</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>